<commit_message>
Añadir formulario informe en sección 2 con resultado comparativo
</commit_message>
<xml_diff>
--- a/app/tables/tabla_newton.xlsx
+++ b/app/tables/tabla_newton.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,13 +465,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0.0701665833531719</v>
       </c>
       <c r="D2" t="n">
-        <v>0.999999700823651</v>
+        <v>0.40499553974338</v>
       </c>
       <c r="E2" t="n">
         <v>1.0005</v>
@@ -482,16 +482,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-2.00000059835288</v>
+        <v>-0.07325273112299439</v>
       </c>
       <c r="C3" t="n">
-        <v>-13.0907111991185</v>
+        <v>-0.0894161133022516</v>
       </c>
       <c r="D3" t="n">
-        <v>14.4161506376861</v>
+        <v>1.44219786502031</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2.36513681424513</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +499,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.09194188503052</v>
+        <v>-0.0112528381325883</v>
       </c>
       <c r="C4" t="n">
-        <v>-2.87337167531518</v>
+        <v>-0.0116329547135328</v>
       </c>
       <c r="D4" t="n">
-        <v>8.09088819941906</v>
+        <v>1.06758004070687</v>
       </c>
       <c r="E4" t="n">
-        <v>0.831599855057283</v>
+        <v>5.50971161762776</v>
       </c>
     </row>
     <row r="5">
@@ -516,16 +516,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.736805142995018</v>
+        <v>-0.0003562736877993</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.430330569290774</v>
+        <v>-0.0003566544881582</v>
       </c>
       <c r="D5" t="n">
-        <v>5.68021148339426</v>
+        <v>1.00213740557536</v>
       </c>
       <c r="E5" t="n">
-        <v>0.481995471138974</v>
+        <v>30.5848139167839</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.661045539580811</v>
+        <v>-3.79889030844877e-07</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0190922105064018</v>
+        <v>-3.79889463791913e-07</v>
       </c>
       <c r="D6" t="n">
-        <v>5.1769221398601</v>
+        <v>1.00000197933424</v>
       </c>
       <c r="E6" t="n">
-        <v>0.114605725139978</v>
+        <v>936.836207081252</v>
       </c>
     </row>
     <row r="7">
@@ -550,16 +550,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.657357593347391</v>
+        <v>-3.18979698465639e-13</v>
       </c>
       <c r="C7" t="n">
-        <v>-4.49701001628e-05</v>
+        <v>-3.18979698465944e-13</v>
       </c>
       <c r="D7" t="n">
-        <v>5.15253565147589</v>
+        <v>0.999999700001916</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0056102588161179</v>
+        <v>1190949.49833022</v>
       </c>
     </row>
     <row r="8">
@@ -567,17 +567,833 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.657348865586304</v>
+        <v>9.569363240798361e-20</v>
       </c>
       <c r="C8" t="n">
-        <v>-2.48887577214418e-10</v>
+        <v>9.569363240798361e-20</v>
       </c>
       <c r="D8" t="n">
-        <v>5.1524779531853</v>
+        <v>0.999999700000002</v>
       </c>
       <c r="E8" t="n">
-        <v>1.32772132801372e-05</v>
-      </c>
+        <v>3333343.98676938</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-2.87080981690177e-26</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-2.87080981690177e-26</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3333333.35258537</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8.61243198333367e-33</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8.61243198333367e-33</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3333333.35311142</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-2.58373035482617e-39</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-2.58373035482617e-39</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3333333.35306326</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>7.751193346564861e-46</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7.751193346564861e-46</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3333333.35194193</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-2.32535868812734e-52</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-2.32535868812734e-52</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3333333.35261312</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6.97607811773455e-59</v>
+      </c>
+      <c r="C14" t="n">
+        <v>6.97607811773455e-59</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3333333.35219346</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>-2.09282405079797e-65</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-2.09282405079797e-65</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3333333.35303496</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>6.27847399913519e-72</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6.27847399913519e-72</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3333333.35287148</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>-1.88354275433081e-78</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-1.88354275433081e-78</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3333333.35186681</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5.65062992697251e-85</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5.65062992697251e-85</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3333333.3517436</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-1.69518947713131e-91</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1.69518947713131e-91</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3333333.35204763</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5.08556992902955e-98</v>
+      </c>
+      <c r="C20" t="n">
+        <v>5.08556992902955e-98</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3333333.3517091</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>-1.525671427662e-104</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-1.525671427662e-104</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3333333.35244688</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>4.57701563132854e-111</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4.57701563132854e-111</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3333333.35136702</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>-1.37310509355541e-117</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-1.37310509355541e-117</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3333333.35220706</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>4.119316492419439e-124</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4.119316492419439e-124</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3333333.35278779</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>-1.23579531182786e-130</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-1.23579531182786e-130</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3333333.35123426</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>3.70738702636011e-137</v>
+      </c>
+      <c r="C26" t="n">
+        <v>3.70738702636011e-137</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3333333.35251987</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.11221643516367e-143</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-1.11221643516367e-143</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3333333.35254209</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>3.33665028630854e-150</v>
+      </c>
+      <c r="C28" t="n">
+        <v>3.33665028630854e-150</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3333333.35349084</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>-1.00099538064761e-156</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-1.00099538064761e-156</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3333333.35179353</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>3.00298702519499e-163</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3.00298702519499e-163</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3333333.35291821</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>-9.00896372857352e-170</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-9.00896372857352e-170</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3333333.35172263</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2.70268991393536e-176</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2.70268991393536e-176</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3333333.35238061</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>-8.10807212637858e-183</v>
+      </c>
+      <c r="C33" t="n">
+        <v>-8.10807212637858e-183</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3333333.35300474</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2.43242235397705e-189</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2.43242235397705e-189</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3333333.3520571</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>-7.29726921108592e-196</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-7.29726921108592e-196</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3333333.35161688</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2.18918140719717e-202</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2.18918140719717e-202</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3333333.35294954</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>-6.56754615266981e-209</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-6.56754615266981e-209</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3333333.3532218</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>1.9702644251223e-215</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1.9702644251223e-215</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3333333.3532257</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>-5.91079501456951e-222</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-5.91079501456951e-222</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3333333.35252754</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1.7732390261617e-228</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1.7732390261617e-228</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3333333.35247132</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>-5.31971864491076e-235</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-5.31971864491076e-235</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3333333.3518117</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1.59591606334192e-241</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1.59591606334192e-241</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3333333.35193525</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>-4.78774959745549e-248</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-4.78774959745549e-248</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3333333.35345075</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1.43632530227017e-254</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1.43632530227017e-254</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3333333.35158376</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>-4.3089771743547e-261</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-4.3089771743547e-261</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3333333.35278804</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1.292693532331e-267</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1.292693532331e-267</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3333333.35340376</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>-3.87808173795635e-274</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-3.87808173795635e-274</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3333333.35263941</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1.16342486365621e-280</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1.16342486365621e-280</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3333333.35269615</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>-3.49027561738075e-287</v>
+      </c>
+      <c r="C49" t="n">
+        <v>-3.49027561738075e-287</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3333333.35307443</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.04708299352463e-293</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1.04708299352463e-293</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3333333.35184348</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>-3.14124990549764e-300</v>
+      </c>
+      <c r="C51" t="n">
+        <v>-3.14124990549764e-300</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3333333.35185167</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>9.423752492319151e-307</v>
+      </c>
+      <c r="C52" t="n">
+        <v>9.423752492319151e-307</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3333333.3514788</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>-2.827126579520802e-313</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-2.827126579520802e-313</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3333333.35256713</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>8.481624942156679e-320</v>
+      </c>
+      <c r="C54" t="n">
+        <v>8.481624942156679e-320</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3333237.96673851</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.999999700000002</v>
+      </c>
+      <c r="E56" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>